<commit_message>
update for new taxotools
</commit_message>
<xml_diff>
--- a/input/Lewis_removed.xlsx
+++ b/input/Lewis_removed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B085EDDF-0072-4FF9-91B2-D1D5B60778FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2F79631-9692-4C57-99BB-FDB5689CE374}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>

</xml_diff>